<commit_message>
Working single set sampling for metabolites using ETC specific expressions for NADH16 and ATPS4r only
</commit_message>
<xml_diff>
--- a/KineticModel/ETC_test.xlsx
+++ b/KineticModel/ETC_test.xlsx
@@ -4,23 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="21075" windowHeight="7485"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21075" windowHeight="7425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ETC_test" sheetId="1" r:id="rId1"/>
     <sheet name="ETC_testC" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
   <si>
     <t>Enzymes</t>
   </si>
@@ -329,6 +328,18 @@
   </si>
   <si>
     <t>pi[e]</t>
+  </si>
+  <si>
+    <t>o2[c]</t>
+  </si>
+  <si>
+    <t>h2o[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2o[e] </t>
+  </si>
+  <si>
+    <t>o2[e]</t>
   </si>
 </sst>
 </file>
@@ -495,14 +506,14 @@
       <sheetName val="red_test2"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
       <sheetData sheetId="8">
         <row r="2">
           <cell r="A2" t="str">
@@ -2648,17 +2659,17 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4458,9 +4469,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="49.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -5235,10 +5251,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5275,19 +5291,39 @@
         <v>1E-4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.27300000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
ACHR code is consistent. Not all samples returned are thermodynamically consistent. Need to reassess or add a filter
</commit_message>
<xml_diff>
--- a/KineticModel/ETC_test.xlsx
+++ b/KineticModel/ETC_test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21075" windowHeight="7425" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21075" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="ETC_test" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -476,6 +481,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4223,7 +4231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4258,7 +4266,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4469,8 +4477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4606,7 +4614,7 @@
         <v>120</v>
       </c>
       <c r="M3" s="5">
-        <v>11.639423575531699</v>
+        <v>20</v>
       </c>
       <c r="N3" s="3" t="str">
         <f>VLOOKUP(A3,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4649,7 +4657,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="5">
-        <v>11.639423575531699</v>
+        <v>20</v>
       </c>
       <c r="N4" s="3" t="str">
         <f>VLOOKUP(A4,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4690,7 +4698,7 @@
         <v>8.5</v>
       </c>
       <c r="M5" s="5">
-        <v>11.639423575531699</v>
+        <v>20</v>
       </c>
       <c r="N5" s="3" t="str">
         <f>VLOOKUP(A5,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4726,7 +4734,7 @@
         <v>9000</v>
       </c>
       <c r="M6" s="7">
-        <v>-11.639423575531699</v>
+        <v>-20</v>
       </c>
       <c r="N6" s="3" t="str">
         <f>VLOOKUP(A6,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4763,7 +4771,7 @@
         <v>268</v>
       </c>
       <c r="M7" s="5">
-        <v>27.772223526897601</v>
+        <v>40</v>
       </c>
       <c r="N7" s="3" t="str">
         <f>VLOOKUP(A7,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4800,7 +4808,7 @@
         <v>654</v>
       </c>
       <c r="M8" s="5">
-        <v>-27.772223526897601</v>
+        <v>-40</v>
       </c>
       <c r="N8" s="3" t="str">
         <f>VLOOKUP(A8,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4836,7 +4844,7 @@
         <v>530</v>
       </c>
       <c r="M9" s="5">
-        <v>-24.294625983764298</v>
+        <v>-40</v>
       </c>
       <c r="N9" s="3" t="str">
         <f>VLOOKUP(A9,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4873,7 +4881,7 @@
         <v>355.79</v>
       </c>
       <c r="M10" s="5">
-        <v>24.294625983764298</v>
+        <v>40</v>
       </c>
       <c r="N10" s="3" t="str">
         <f>VLOOKUP(A10,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4910,7 +4918,7 @@
         <v>2540</v>
       </c>
       <c r="M11" s="5">
-        <v>-8.5077261088811902</v>
+        <v>-20</v>
       </c>
       <c r="N11" s="3" t="str">
         <f>VLOOKUP(A11,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4950,7 +4958,7 @@
         <v>200</v>
       </c>
       <c r="M12" s="5">
-        <v>-43.153531211344998</v>
+        <v>40</v>
       </c>
       <c r="N12" s="3" t="str">
         <f>VLOOKUP(A12,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -4981,7 +4989,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="5">
-        <v>8.39</v>
+        <v>140</v>
       </c>
       <c r="N13" s="3"/>
     </row>
@@ -5012,7 +5020,7 @@
         <v>5130</v>
       </c>
       <c r="M14" s="5">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="N14" s="3" t="str">
         <f>VLOOKUP(A14,[2]reactions!$A$1:$E$96,5,FALSE)</f>
@@ -5041,7 +5049,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="5">
-        <v>46.7215117629625</v>
+        <v>40</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>67</v>
@@ -5068,7 +5076,7 @@
         <v>2</v>
       </c>
       <c r="M16" s="5">
-        <v>-13.3040694607334</v>
+        <v>60</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" t="s">
@@ -5093,7 +5101,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="5">
-        <v>23.3607558814812</v>
+        <v>20</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" t="s">
@@ -5119,7 +5127,7 @@
         <v>100</v>
       </c>
       <c r="M18" s="5">
-        <v>8.5514960440672301</v>
+        <v>0</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="6" t="s">
@@ -5147,7 +5155,7 @@
         <v>2540</v>
       </c>
       <c r="M19" s="5">
-        <v>-8.5077261088811902</v>
+        <v>-40</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" t="s">
@@ -5165,7 +5173,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="5">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="N20" s="3"/>
     </row>
@@ -5195,7 +5203,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="5">
-        <v>63.607356573910501</v>
+        <v>40</v>
       </c>
       <c r="N22" s="3"/>
     </row>
@@ -5210,7 +5218,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="5">
-        <v>13.304069460733899</v>
+        <v>-60</v>
       </c>
       <c r="N23" s="3"/>
     </row>
@@ -5225,7 +5233,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="5">
-        <v>-8.5514960440672301</v>
+        <v>0</v>
       </c>
       <c r="N24" s="3"/>
     </row>
@@ -5240,7 +5248,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="5">
-        <v>-23.3607558814812</v>
+        <v>-20</v>
       </c>
       <c r="N25" s="3"/>
     </row>
@@ -5253,7 +5261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
All sampling changes are complete and working for ETC additions
</commit_message>
<xml_diff>
--- a/KineticModel/ETC_test.xlsx
+++ b/KineticModel/ETC_test.xlsx
@@ -4477,8 +4477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5262,7 +5262,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes to buildmodel to do repeated sampling for inconsistent reactions - not working and leads to infinite loops, need to check parameters for FBA
</commit_message>
<xml_diff>
--- a/KineticModel/ETC_test.xlsx
+++ b/KineticModel/ETC_test.xlsx
@@ -4477,13 +4477,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="49.5703125" customWidth="1"/>
+    <col min="15" max="15" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
@@ -4695,7 +4696,7 @@
       </c>
       <c r="H5" s="6"/>
       <c r="I5">
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
       <c r="M5" s="5">
         <v>20</v>

</xml_diff>

<commit_message>
Can obtain feasible models for E. coli, Remove commented sections from buildmodel.m
</commit_message>
<xml_diff>
--- a/KineticModel/ETC_test.xlsx
+++ b/KineticModel/ETC_test.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="21075" windowHeight="7425"/>
   </bookViews>
@@ -19,12 +14,12 @@
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>Enzymes</t>
   </si>
@@ -345,6 +340,9 @@
   </si>
   <si>
     <t>o2[e]</t>
+  </si>
+  <si>
+    <t>0.2331,0.1316,0.1675</t>
   </si>
 </sst>
 </file>
@@ -4231,7 +4229,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4266,7 +4264,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4478,7 +4476,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection sqref="A1:U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4704,6 +4702,9 @@
       <c r="N5" s="3" t="str">
         <f>VLOOKUP(A5,[2]reactions!$A$1:$E$96,5,FALSE)</f>
         <v>4.1.2.13</v>
+      </c>
+      <c r="O5" t="s">
+        <v>100</v>
       </c>
       <c r="S5" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Chnages to make buildmodels.m functional with new ETCflux.m and other corrections to Tkientics.m
</commit_message>
<xml_diff>
--- a/KineticModel/ETC_test.xlsx
+++ b/KineticModel/ETC_test.xlsx
@@ -15,11 +15,12 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>Enzymes</t>
   </si>
@@ -478,9 +479,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -4475,7 +4473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection sqref="A1:U25"/>
     </sheetView>
   </sheetViews>
@@ -5123,10 +5121,10 @@
         <v>0</v>
       </c>
       <c r="I18" s="6">
-        <v>100</v>
+        <v>1.3299999999999999E-2</v>
       </c>
       <c r="J18" s="6">
-        <v>100</v>
+        <v>1.3299999999999999E-2</v>
       </c>
       <c r="M18" s="5">
         <v>0</v>
@@ -5143,9 +5141,6 @@
       <c r="B19" s="12"/>
       <c r="C19" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
       </c>
       <c r="E19">
         <v>0</v>

</xml_diff>

<commit_message>
Accomodate difference in number of variables and number of model metabolites in Integratemodel.m
</commit_message>
<xml_diff>
--- a/KineticModel/ETC_test.xlsx
+++ b/KineticModel/ETC_test.xlsx
@@ -15,7 +15,6 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -4473,9 +4472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:U25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
changes to modelgen.m and CKinetics.m to allow regulation
</commit_message>
<xml_diff>
--- a/KineticModel/ETC_test.xlsx
+++ b/KineticModel/ETC_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21075" windowHeight="7425"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="21075" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="ETC_test" sheetId="1" r:id="rId1"/>
@@ -509,14 +509,14 @@
       <sheetName val="red_test2"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
       <sheetData sheetId="8">
         <row r="2">
           <cell r="A2" t="str">
@@ -2662,17 +2662,17 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4472,7 +4472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:U25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Developing generic flux production envelopes
</commit_message>
<xml_diff>
--- a/KineticModel/ETC_test.xlsx
+++ b/KineticModel/ETC_test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\Courses\CHE1125Project\IntegratedModels\KineticModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="180" windowWidth="21075" windowHeight="7365"/>
   </bookViews>
@@ -14,7 +19,7 @@
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -479,6 +484,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4226,7 +4234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4261,7 +4269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4472,8 +4480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:U25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>